<commit_message>
update: 0 weight on SE3_SWL and SE3_FS
</commit_message>
<xml_diff>
--- a/data/map_atceFB-ig107.xlsx
+++ b/data/map_atceFB-ig107.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="332" documentId="8_{E773FC41-18B2-4904-BDD2-06551D0A29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC51B640-1441-48A5-80AF-AE449219286B}"/>
+  <xr:revisionPtr revIDLastSave="335" documentId="8_{E773FC41-18B2-4904-BDD2-06551D0A29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DA2BF95-12B6-4EA2-9338-A3EC0706F0FE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
+    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="1" r:id="rId1"/>
@@ -306,7 +306,7 @@
     <t>topology_atceFB</t>
   </si>
   <si>
-    <t>'2024-08-12</t>
+    <t>'2024-12-13</t>
   </si>
 </sst>
 </file>
@@ -742,17 +742,17 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="23.28515625" customWidth="1"/>
+    <col min="1" max="8" width="23.26953125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
+    <col min="10" max="10" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
@@ -784,12 +784,12 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="2">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>88</v>
@@ -801,7 +801,7 @@
         <v>87</v>
       </c>
       <c r="F2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G2" t="s">
         <v>75</v>
@@ -816,15 +816,15 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
@@ -844,14 +844,14 @@
       <selection activeCell="A66" sqref="A66:XFD66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.1796875" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>63</v>
       </c>
@@ -859,7 +859,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -867,7 +867,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -875,7 +875,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -883,7 +883,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>39</v>
       </c>
@@ -892,7 +892,7 @@
       </c>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -901,7 +901,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>41</v>
       </c>
@@ -910,7 +910,7 @@
       </c>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>76</v>
       </c>
@@ -919,7 +919,7 @@
       </c>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -927,7 +927,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -935,7 +935,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -943,7 +943,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -952,7 +952,7 @@
       </c>
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -960,7 +960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -969,7 +969,7 @@
       </c>
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -978,7 +978,7 @@
       </c>
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -986,7 +986,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>48</v>
       </c>
@@ -994,7 +994,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>78</v>
       </c>
@@ -1002,7 +1002,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>3</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>5</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1026,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>6</v>
       </c>
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1042,7 +1042,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1050,7 +1050,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>50</v>
       </c>
@@ -1058,7 +1058,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>51</v>
       </c>
@@ -1067,7 +1067,7 @@
       </c>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1086,7 +1086,7 @@
       <c r="D28" s="4"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>62</v>
       </c>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>53</v>
       </c>
@@ -1103,7 +1103,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>11</v>
       </c>
@@ -1120,7 +1120,7 @@
       </c>
       <c r="D32" s="4"/>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>12</v>
       </c>
@@ -1129,7 +1129,7 @@
       </c>
       <c r="D33" s="4"/>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>13</v>
       </c>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="D34" s="4"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -1154,7 +1154,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>15</v>
       </c>
@@ -1162,7 +1162,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>16</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>17</v>
       </c>
@@ -1179,7 +1179,7 @@
       </c>
       <c r="D39" s="4"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1187,7 +1187,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>19</v>
       </c>
@@ -1195,7 +1195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>20</v>
       </c>
@@ -1203,7 +1203,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>21</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>22</v>
       </c>
@@ -1219,7 +1219,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>23</v>
       </c>
@@ -1227,7 +1227,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>24</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>25</v>
       </c>
@@ -1243,7 +1243,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>27</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -1267,7 +1267,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -1275,7 +1275,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -1291,7 +1291,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>30</v>
       </c>
@@ -1299,7 +1299,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>80</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>31</v>
       </c>
@@ -1315,7 +1315,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>81</v>
       </c>
@@ -1324,7 +1324,7 @@
       </c>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -1332,7 +1332,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -1340,7 +1340,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -1349,7 +1349,7 @@
       </c>
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>33</v>
       </c>
@@ -1358,7 +1358,7 @@
       </c>
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>34</v>
       </c>
@@ -1367,7 +1367,7 @@
       </c>
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -1385,7 +1385,7 @@
       </c>
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -1394,7 +1394,7 @@
       </c>
       <c r="D65" s="4"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D70" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix DK1-DK2 border reversal
</commit_message>
<xml_diff>
--- a/data/map_atceFB-ig107.xlsx
+++ b/data/map_atceFB-ig107.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nordicrsc-my.sharepoint.com/personal/jlm_nordic-rcc_net/Documents/Dokumenter/topology/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="335" documentId="8_{E773FC41-18B2-4904-BDD2-06551D0A29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2DA2BF95-12B6-4EA2-9338-A3EC0706F0FE}"/>
+  <xr:revisionPtr revIDLastSave="355" documentId="8_{E773FC41-18B2-4904-BDD2-06551D0A29DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F272DDA3-B63F-4288-B444-4D0FE494D6B8}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-5490" windowWidth="38640" windowHeight="21120" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{879DBF62-5915-4E1B-BB81-2834436B8A2E}"/>
   </bookViews>
   <sheets>
     <sheet name="metaData" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="79">
   <si>
     <t>DK1-DK2</t>
   </si>
@@ -240,24 +240,6 @@
     <t>mapName</t>
   </si>
   <si>
-    <t>TopologyFile1</t>
-  </si>
-  <si>
-    <t>TopologyFile2</t>
-  </si>
-  <si>
-    <t>topology1Name</t>
-  </si>
-  <si>
-    <t>topology1version</t>
-  </si>
-  <si>
-    <t>topology2Name</t>
-  </si>
-  <si>
-    <t>topology2version</t>
-  </si>
-  <si>
     <t>mapVersion</t>
   </si>
   <si>
@@ -267,9 +249,6 @@
     <t>jlm@nordic-rcc.net</t>
   </si>
   <si>
-    <t>topology_ig107.JSON</t>
-  </si>
-  <si>
     <t>DK1-DK1_KS</t>
   </si>
   <si>
@@ -294,19 +273,10 @@
     <t>mapCreatedDate</t>
   </si>
   <si>
-    <t>topology_atceFB.JSON</t>
-  </si>
-  <si>
-    <t>topology_ig107</t>
-  </si>
-  <si>
     <t>map_atceFB-ig107</t>
   </si>
   <si>
-    <t>topology_atceFB</t>
-  </si>
-  <si>
-    <t>'2024-12-13</t>
+    <t>2025-04-25</t>
   </si>
 </sst>
 </file>
@@ -371,12 +341,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -739,98 +712,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A7284C-B5FB-484E-A2B3-0244298D3E3F}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="8" width="23.26953125" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.26953125" style="5" customWidth="1"/>
+    <col min="3" max="8" width="23.26953125" customWidth="1"/>
     <col min="9" max="9" width="16" customWidth="1"/>
     <col min="10" max="10" width="23.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
-      <c r="B1" t="s">
-        <v>72</v>
+      <c r="B1" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="D1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B2" s="6">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" t="s">
-        <v>70</v>
-      </c>
-      <c r="I1" t="s">
-        <v>71</v>
-      </c>
-      <c r="J1" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="2">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="2">
-        <v>2</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B5" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="I2" s="2"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="6"/>
       <c r="C5" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B8" s="2"/>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8" s="6"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="B9" s="1"/>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9" s="7"/>
       <c r="C9" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" xr:uid="{7ABA21AD-F2F3-46BA-895E-92C397578E09}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7ABA21AD-F2F3-46BA-895E-92C397578E09}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -840,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D153D6-6422-49A5-92A2-7897A0750DDC}">
   <dimension ref="A1:I70"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66:XFD66"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -912,19 +853,19 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -940,7 +881,7 @@
         <v>43</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -957,7 +898,7 @@
         <v>45</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -996,10 +937,10 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.35">
@@ -1148,10 +1089,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.35">
@@ -1301,10 +1242,10 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
@@ -1317,10 +1258,10 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D57" s="4"/>
     </row>
@@ -1369,10 +1310,10 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D63" s="4"/>
     </row>

</xml_diff>